<commit_message>
Actualizacion de codigo y documentos de apoyo
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 07 - Colisiones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="508" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4EB7BB55-9FF2-4D50-B29C-4A9592E97488}"/>
+  <xr:revisionPtr revIDLastSave="511" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A6E5986-5D76-40E6-8BB6-4E7550720C79}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" tabRatio="767" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-2127" yWindow="7073" windowWidth="4267" windowHeight="2354" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab7" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab7'!$A$9:$C$9</c:f>
+              <c:f>'Datos Lab7'!$A$8:$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -575,10 +575,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab7'!$B$3:$B$6</c:f>
+              <c:f>'Datos Lab7'!$B$3:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -586,9 +586,6 @@
                   <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
@@ -596,10 +593,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab7'!$C$3:$C$6</c:f>
+              <c:f>'Datos Lab7'!$C$3:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>45</c:v>
                 </c:pt>
@@ -607,9 +604,6 @@
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
@@ -627,7 +621,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab7'!$A$9:$C$9</c:f>
+              <c:f>'Datos Lab7'!$A$8:$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -707,10 +701,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab7'!$B$11:$B$14</c:f>
+              <c:f>'Datos Lab7'!$B$10:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -720,18 +714,15 @@
                 <c:pt idx="2">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>160</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab7'!$C$11:$C$14</c:f>
+              <c:f>'Datos Lab7'!$C$10:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>90</c:v>
                 </c:pt>
@@ -740,9 +731,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1649,7 +1637,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CA07E00A-1DDB-47A3-B681-B59870FF7EA9}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1690,8 +1678,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A2:C6" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A2:C5" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Consumo de Datos [kB]" dataDxfId="6"/>
@@ -1702,8 +1690,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:C14" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A10:C14" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A9:C12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A9:C12" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Consumo de Datos [kB]" dataDxfId="1"/>
@@ -2010,10 +1998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2043,7 +2031,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="B3" s="2">
         <v>100</v>
@@ -2065,93 +2053,71 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="B5" s="2">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C5" s="2">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A6" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>115</v>
-      </c>
-      <c r="C6" s="2">
-        <v>75</v>
-      </c>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="A10" s="2">
         <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2">
+        <v>120</v>
+      </c>
+      <c r="C11" s="2">
         <v>100</v>
-      </c>
-      <c r="C11" s="2">
-        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="C12" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A13" s="2">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2">
-        <v>140</v>
-      </c>
-      <c r="C13" s="2">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A14" s="2">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2">
-        <v>160</v>
-      </c>
-      <c r="C14" s="2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" ht="14.7" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="21" ht="14.7" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -2373,18 +2339,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2407,14 +2373,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -2429,4 +2387,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>